<commit_message>
Eaegle-Files mit Versionsnummern versehen und Version 2.0 hinzugefügt
</commit_message>
<xml_diff>
--- a/eagle/main_bom.xlsx
+++ b/eagle/main_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="265">
   <si>
     <t>Part</t>
   </si>
@@ -809,6 +809,12 @@
   </si>
   <si>
     <t>Cinch-Buchse</t>
+  </si>
+  <si>
+    <t>Ersatztyp TORX1952, lieferbar bei Segor</t>
+  </si>
+  <si>
+    <t>durch Step-Down Wandler ersetzen, MAX1921</t>
   </si>
 </sst>
 </file>
@@ -1705,10 +1711,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2142,7 +2148,7 @@
         <v>0.11399999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" s="2">
         <v>3</v>
       </c>
@@ -2169,7 +2175,7 @@
         <v>0.11399999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <v>4</v>
       </c>
@@ -2196,7 +2202,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -2223,7 +2229,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="2">
         <v>2</v>
       </c>
@@ -2247,7 +2253,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21" s="2">
         <v>3</v>
       </c>
@@ -2271,7 +2277,7 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -2292,7 +2298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -2319,7 +2325,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -2346,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -2393,8 +2399,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="2">
         <v>1</v>
       </c>
@@ -2421,7 +2430,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" s="2">
         <v>1</v>
       </c>
@@ -2445,7 +2454,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29" s="2">
         <v>2</v>
       </c>
@@ -2465,8 +2474,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="30">
+      <c r="I29" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30">
       <c r="A30" s="2">
         <v>5</v>
       </c>
@@ -2493,7 +2505,7 @@
         <v>0.35000000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31" s="2">
         <v>1</v>
       </c>
@@ -2517,7 +2529,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30">
+    <row r="32" spans="1:9" ht="30">
       <c r="A32" s="2">
         <v>2</v>
       </c>

</xml_diff>